<commit_message>
updates to directional solidification yaml schema
</commit_message>
<xml_diff>
--- a/directional_solidification_IKZ/G1_IKZ_NSI_23-Manual_Protocol.xlsx
+++ b/directional_solidification_IKZ/G1_IKZ_NSI_23-Manual_Protocol.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="80">
   <si>
-    <t xml:space="preserve">Note: format these cells as text not as date to avoid misformatting</t>
+    <t xml:space="preserve"># Note: format these cells as text not as date to avoid misformatting</t>
   </si>
   <si>
     <t xml:space="preserve">CO</t>
@@ -38,7 +38,7 @@
       H1-9 </t>
   </si>
   <si>
-    <t xml:space="preserve">hh:mm:ss+00</t>
+    <t xml:space="preserve"># hh:mm:ss+00</t>
   </si>
   <si>
     <t xml:space="preserve">Liter / h</t>
@@ -254,7 +254,7 @@
     <t xml:space="preserve">Notes</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-19-03 13:10:00+01</t>
+    <t xml:space="preserve">2023-03-19 13:10:00+01</t>
   </si>
   <si>
     <t xml:space="preserve">2</t>
@@ -576,12 +576,12 @@
   <dimension ref="A1:BN6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.27"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="5.98"/>

</xml_diff>